<commit_message>
add min and max column on the product template
</commit_message>
<xml_diff>
--- a/storage/app/Files/product_import_template.xlsx
+++ b/storage/app/Files/product_import_template.xlsx
@@ -8,10 +8,10 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$U$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$U$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t xml:space="preserve">STATUS</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t xml:space="preserve">Max Discount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum Stock Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum Stock Level</t>
   </si>
   <si>
     <t xml:space="preserve">active</t>
@@ -222,28 +228,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -260,15 +270,15 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF3D3D3D"/>
-          <bgColor rgb="FFFFFFFF"/>
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -280,8 +290,114 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -290,190 +406,198 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="O4" activeCellId="0" sqref="O4"/>
+      <selection pane="bottomLeft" activeCell="R12" activeCellId="0" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="19.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="52.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="47.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="19.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="15.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="14.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="14.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="21.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="21.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="1" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="AMI1" s="1"/>
+      <c r="AMJ1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="G2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="H2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="I2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="J2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="1" t="n">
         <v>11.5</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="M2" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="N2" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="0" t="n">
+      <c r="N2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="P2" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="0" t="n">
+      <c r="P2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="B3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="G3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="I3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="J3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M3" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="N3" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="O3" s="0" t="n">
+      <c r="N3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="P3" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q3" s="0" t="n">
+      <c r="P3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -524,7 +648,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:U1"/>
+  <autoFilter ref="A1:U3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
add part no. column on the product template
</commit_message>
<xml_diff>
--- a/storage/app/Files/product_import_template.xlsx
+++ b/storage/app/Files/product_import_template.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t xml:space="preserve">STATUS</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t xml:space="preserve">Maximum Stock Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part Number</t>
   </si>
   <si>
     <t xml:space="preserve">active</t>
@@ -406,7 +409,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="R12" activeCellId="0" sqref="R12"/>
+      <selection pane="bottomLeft" activeCell="T11" activeCellId="0" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -425,10 +428,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="13.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="14.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="14.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="21.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="14.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="21.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="27.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="1" width="9.14"/>
   </cols>
   <sheetData>
@@ -490,44 +493,46 @@
       <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3"/>
+      <c r="T1" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="U1" s="3"/>
       <c r="AMI1" s="1"/>
       <c r="AMJ1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L2" s="1" t="n">
         <v>11.5</v>
@@ -536,13 +541,13 @@
         <v>22</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O2" s="1" t="n">
         <v>22</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q2" s="1" t="n">
         <v>1</v>
@@ -550,37 +555,37 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L3" s="1" t="n">
         <v>69</v>
@@ -589,13 +594,13 @@
         <v>100</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O3" s="1" t="n">
         <v>22</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q3" s="1" t="n">
         <v>2</v>

</xml_diff>